<commit_message>
fixes & integration tests (write)
</commit_message>
<xml_diff>
--- a/tests/integration_write.xlsx
+++ b/tests/integration_write.xlsx
@@ -2,20 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10118"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fz/Dev/xlwings/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709C4FBB-F001-1A40-AB54-9173E4FEDDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB1D014-89D1-5240-8FEE-D221E512F2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="500" windowWidth="34880" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="960" yWindow="500" windowWidth="17440" windowHeight="10960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="18" r:id="rId2"/>
+    <sheet name="Autofit" sheetId="19" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -55,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>string</t>
   </si>
@@ -64,13 +66,52 @@
   </si>
   <si>
     <t>actual</t>
+  </si>
+  <si>
+    <t>Type Conversion</t>
+  </si>
+  <si>
+    <t>Number Format</t>
+  </si>
+  <si>
+    <t>(Ctrl-Alt-F9)</t>
+  </si>
+  <si>
+    <t>rows</t>
+  </si>
+  <si>
+    <t>cols</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Hyperlink</t>
+  </si>
+  <si>
+    <t>xlwings</t>
+  </si>
+  <si>
+    <t>Active Sheet: Changed</t>
+  </si>
+  <si>
+    <t>Renamed Sheet: Sheet2 -&gt; Changed (contains text)</t>
+  </si>
+  <si>
+    <t>Autofit</t>
+  </si>
+  <si>
+    <t>Clear Contents</t>
+  </si>
+  <si>
+    <t>xxxxx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +134,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,6 +176,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3DBAC1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -123,10 +192,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -143,12 +214,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="22" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -163,6 +239,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF3DBAC1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -477,6 +558,9 @@
   <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </wetp:taskpane>
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+  </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
@@ -502,117 +586,356 @@
 </we:webextension>
 </file>
 
+<file path=xl/webextensions/webextension3.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{820A6B7C-A8FF-F24E-8A7E-BDC66C7D640E}">
+  <we:reference id="wa200005075" version="1.0.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="WA200005075" version="1.0.0.0" store="WA200005075" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="C1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="7" t="s">
+    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="D2" s="1"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="b">
-        <f>AND(_xlfn.ANCHORARRAY(F4))</f>
-        <v>0</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="3">
+        <f>AND(_xlfn.ANCHORARRAY(G4))</f>
+        <v>0</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" s="3">
         <v>-1</v>
       </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" t="b" cm="1">
-        <f t="array" ref="F4:G7">B4:C7=D4:E7</f>
-        <v>0</v>
-      </c>
-      <c r="G4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="3">
+      <c r="D4" s="3">
+        <v>1</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" t="b" cm="1">
+        <f t="array" ref="G4:H7">C4:D7=E4:F7</f>
+        <v>0</v>
+      </c>
+      <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C5" s="3">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" t="b">
-        <v>0</v>
-      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
       <c r="G5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
+      <c r="H5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C6" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
       <c r="G6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C7" s="4">
         <v>44378</v>
       </c>
-      <c r="C7" s="5">
+      <c r="D7" s="5">
         <v>44561.982777777775</v>
       </c>
-      <c r="D7" s="9"/>
       <c r="E7" s="10"/>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
+      <c r="F7" s="10"/>
       <c r="G7" t="b">
         <v>0</v>
       </c>
+      <c r="H7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="b">
+        <f ca="1">AND(G9:H10)</f>
+        <v>0</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2</v>
+      </c>
+      <c r="E9" s="10">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10">
+        <v>2</v>
+      </c>
+      <c r="G9" t="b" cm="1">
+        <f t="array" aca="1" ref="G9" ca="1">CELL("format",E9) = "P0"</f>
+        <v>0</v>
+      </c>
+      <c r="H9" t="b" cm="1">
+        <f t="array" aca="1" ref="H9" ca="1">CELL("format",F9) = "P0"</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8">
+        <v>3</v>
+      </c>
+      <c r="D10" s="8">
+        <v>4</v>
+      </c>
+      <c r="E10" s="10">
+        <v>3</v>
+      </c>
+      <c r="F10" s="10">
+        <v>4</v>
+      </c>
+      <c r="G10" t="b" cm="1">
+        <f t="array" aca="1" ref="G10" ca="1">CELL("format",E10) = "P0"</f>
+        <v>0</v>
+      </c>
+      <c r="H10" t="b" cm="1">
+        <f t="array" aca="1" ref="H10" ca="1">CELL("format",F10) = "P0"</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="b">
+        <f>G14=TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="b">
+        <f>E14=D14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="b">
+        <f>AND(_xlfn.ANCHORARRAY(G16))</f>
+        <v>0</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="b" cm="1">
+        <f t="array" ref="G16:H17">C16:D17=E16:F17</f>
+        <v>0</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="9" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A1048576">
+  <conditionalFormatting sqref="A1:B1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E14" r:id="rId1" tooltip="xw homepage" xr:uid="{544ACF97-C1A4-E24A-A1F0-453AFFC09E1F}"/>
+    <hyperlink ref="D14" r:id="rId2" tooltip="xw homepage" xr:uid="{05AC7D58-7BDC-CC45-B621-AE100AB454F7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{051EE511-2883-1E42-8761-2DA62FE05B86}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653321CA-2FE0-DC4E-8C0A-3CE881BD82AD}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="8" width="13.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>